<commit_message>
commit after a long time
</commit_message>
<xml_diff>
--- a/app/src/main/assets/kontrola.xlsx
+++ b/app/src/main/assets/kontrola.xlsx
@@ -71,8 +71,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -175,7 +176,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -185,6 +186,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -310,384 +315,384 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="3"/>
       <c r="L3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3" t="s">
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="125.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="3"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
+      <c r="A7" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="n">
+      <c r="A12" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="n">
+      <c r="A13" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="n">
+      <c r="A14" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="n">
+      <c r="A15" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="n">
+      <c r="A16" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="n">
+      <c r="A17" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="n">
+      <c r="A18" s="6" t="n">
         <v>12</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="n">
+      <c r="A19" s="6" t="n">
         <v>13</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="n">
+      <c r="A20" s="6" t="n">
         <v>14</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="n">
+      <c r="A21" s="6" t="n">
         <v>15</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="n">
+      <c r="A22" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="n">
+      <c r="A23" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="n">
+      <c r="A24" s="8" t="n">
         <v>18</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="n">
+      <c r="A25" s="8" t="n">
         <v>19</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="n">
+      <c r="A26" s="8" t="n">
         <v>20</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>